<commit_message>
Correzioni dei TC riguardanti il timed out
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="263">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1646,6 +1646,27 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1667,27 +1688,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1984,18 +1984,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="130.140625" style="45" customWidth="1"/>
+    <col min="1" max="1" width="130.140625" style="33" customWidth="1"/>
     <col min="2" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2033,7 +2033,7 @@
       <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4148,10 +4148,10 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P51" sqref="P51"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4190,12 +4190,12 @@
       <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -4213,14 +4213,14 @@
       <c r="T2" s="14"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="42"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -4238,12 +4238,12 @@
       <c r="T3" s="14"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="43" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="3"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -4262,12 +4262,12 @@
       <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="42"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -4285,8 +4285,8 @@
       <c r="T5" s="14"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="15"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -4513,7 +4513,7 @@
       <c r="G12" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="34" t="s">
         <v>202</v>
       </c>
       <c r="I12" s="23" t="s">
@@ -4557,7 +4557,7 @@
       <c r="G13" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="H13" s="36" t="s">
         <v>205</v>
       </c>
       <c r="I13" s="23" t="s">
@@ -4601,10 +4601,10 @@
       <c r="G14" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="H14" s="50" t="s">
+      <c r="H14" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="35" t="s">
         <v>209</v>
       </c>
       <c r="J14" s="24" t="s">
@@ -4645,7 +4645,7 @@
       <c r="G15" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="H15" s="49" t="s">
+      <c r="H15" s="37" t="s">
         <v>211</v>
       </c>
       <c r="I15" s="23" t="s">
@@ -4983,15 +4983,17 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
-      <c r="J22" s="24"/>
+      <c r="J22" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
-      <c r="N22" s="24" t="s">
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
       <c r="R22" s="25" t="s">
         <v>80</v>
@@ -5021,15 +5023,17 @@
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
+      <c r="J23" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
-      <c r="N23" s="24" t="s">
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
       <c r="Q23" s="24"/>
       <c r="R23" s="25" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Rifatti i TC con ID  [22, 23, 16, 17, 18, 19, 20, 21] come richiesto da mail del 19/04/2023. I TC hanno tutti restituito 201
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
@@ -982,15 +982,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>2023-02-06T16:48:29Z</t>
-  </si>
-  <si>
-    <t>ce943e4442bb2265</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.af44698f5243cd06a07244c5bbf19d9f62b46a5d04e74454a3a4f5173499b9de.9106321210^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>subject_application_vendor: CONSORZIO METIS</t>
   </si>
   <si>
@@ -1000,69 +991,6 @@
     <t xml:space="preserve"> subject_application_version: V.23</t>
   </si>
   <si>
-    <t>2023-02-06T17:17:05Z</t>
-  </si>
-  <si>
-    <t>164b9e8c88c4194c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.11cdc6d7029c467805ea83b5d928e53f2dfd876a74ccf257b77bb315a437305d.2ca2262a70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T10:37:44Z</t>
-  </si>
-  <si>
-    <t>6424e05331d59204</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.f7fbdb8518942fc7623480d4a9127da0e5129e690004c9564b7dd3f99f312b48.b0239a7138^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T10:53:54Z</t>
-  </si>
-  <si>
-    <t>e994003eb755a932</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.77c5c58b4930b23b1dbbb36ba7625bcd8e2444a7c80a3918635fb3e2e5502b46.8733c9c496^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T10:10:37Z</t>
-  </si>
-  <si>
-    <t>0188b03878495dd0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.b3cdf19ad7da26c8809fd833baae57350d40fb497ae8da21ea2164efc250af62.fb9efd7031^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T11:18:00Z</t>
-  </si>
-  <si>
-    <t>8e864dfd815482f4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.cee9f713d63dd608714e7dd54350ec0f5f9d555eb2290efb31409ac17c4f565c.3cf226db35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-14T16:49:14Z</t>
-  </si>
-  <si>
-    <t>bf31f594b311b152</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.0d79c9ac7146e99d03ecfbda28d52593eb90ca9279c6ecd4b3bd358dff158a67.49c8cd73a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T13:24:19Z</t>
-  </si>
-  <si>
-    <t>3282001096a84fd2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.f70d3c17258416b9a31076313afb5e2cc1bfd88fb19a218048b0bcd6aa5c40b3.048ca9593f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-02-07T11:02:43Z</t>
   </si>
   <si>
@@ -1193,13 +1121,85 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.21b4a6d4582e24e59a93e58b02d7ebb369c2a92f78e2e4239541bddbbe73b2c6.27e3fb0981^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:05:12Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.b86fff0452a3aae8a0acd566eec171d95b3908c07503e1495e2d138be9134225.abfed3901a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6b179620ec85dbe0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.175b8f108bcc5ea17a732c6fbeb18b7025e0cc3232964d8942ddb53cdb17fd9a.63a38abbb5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a3cf3b5c19272cdd</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:10:15Z</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:08:23Z</t>
+  </si>
+  <si>
+    <t>1428c712f8916a76</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.13fe600756d537bf541df2ed8c872776d3a7fa45bb3014fce93ed81b0968b614.7ff65771ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:12:49Z</t>
+  </si>
+  <si>
+    <t>92303229cb0e0298</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.568a98c8082cbe60f8ad265ba25a3a71120a9dc6a69f8793dbb9dd13dacb6437.dda60a4541^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.96802c60667a485296ce409c1a180571e474f7787085fd3b0f50a345f90966f5.cb8d44fb06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5831b11d953c9a13</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:21:27Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.13990634ffd3495cc662e1513675d9ed5a5ba6e0da7d67623afd2dcbd629321a.6057a07857^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>fa03e049a589094f</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:27:25Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.f2abc4b7f41e4b49e1c5b4048b57032d0e5b97db37d451f62ad478b9d7892119.f96f04e4a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>77e31ff1e4d108b6</t>
+  </si>
+  <si>
+    <t>2023-04-20T13:56:44Z</t>
+  </si>
+  <si>
+    <t>2023-04-20T14:05:52Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.04fb2bc081906f3c5dc64680842ca0659b30570f241c9da84a00826eafc3c164.edd89baa12^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6e894a3baaf6bcd2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1253,6 +1253,13 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1557,7 +1564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1658,9 +1665,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1688,6 +1692,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4148,10 +4158,10 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4190,12 +4200,12 @@
       <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="42"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -4213,14 +4223,14 @@
       <c r="T2" s="14"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="41"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -4238,12 +4248,12 @@
       <c r="T3" s="14"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="42"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="41"/>
       <c r="E4" s="3"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -4262,12 +4272,12 @@
       <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="42"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="41"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -4285,8 +4295,8 @@
       <c r="T5" s="14"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="15"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -4420,16 +4430,16 @@
         <v>56</v>
       </c>
       <c r="F10" s="22">
-        <v>44963</v>
+        <v>45036</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>192</v>
+        <v>253</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>193</v>
+        <v>252</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>194</v>
+        <v>251</v>
       </c>
       <c r="J10" s="24" t="s">
         <v>80</v>
@@ -4447,7 +4457,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="150.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>17</v>
       </c>
@@ -4463,17 +4473,17 @@
       <c r="E11" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="22">
-        <v>44963</v>
+      <c r="F11" s="50">
+        <v>45036</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>198</v>
+        <v>256</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>199</v>
+        <v>255</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>80</v>
@@ -4491,7 +4501,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="150.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>18</v>
       </c>
@@ -4507,17 +4517,17 @@
       <c r="E12" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="22">
-        <v>44964</v>
+      <c r="F12" s="50">
+        <v>45036</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>203</v>
+        <v>257</v>
       </c>
       <c r="J12" s="24" t="s">
         <v>80</v>
@@ -4535,7 +4545,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="135.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>19</v>
       </c>
@@ -4551,17 +4561,17 @@
       <c r="E13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="22">
-        <v>44964</v>
+      <c r="F13" s="50">
+        <v>45036</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="H13" s="36" t="s">
-        <v>205</v>
+        <v>260</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>262</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>206</v>
+        <v>261</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>80</v>
@@ -4596,16 +4606,16 @@
         <v>64</v>
       </c>
       <c r="F14" s="22">
-        <v>44960</v>
+        <v>45036</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>208</v>
+        <v>239</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>241</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="J14" s="24" t="s">
         <v>80</v>
@@ -4640,16 +4650,16 @@
         <v>66</v>
       </c>
       <c r="F15" s="22">
-        <v>44960</v>
+        <v>45036</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="H15" s="37" t="s">
-        <v>211</v>
+        <v>245</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>246</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="J15" s="24" t="s">
         <v>80</v>
@@ -4684,16 +4694,16 @@
         <v>68</v>
       </c>
       <c r="F16" s="22">
-        <v>44971</v>
+        <v>45036</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="J16" s="24" t="s">
         <v>80</v>
@@ -4728,16 +4738,16 @@
         <v>70</v>
       </c>
       <c r="F17" s="22">
-        <v>44960</v>
+        <v>45036</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="H17" s="23" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="J17" s="24" t="s">
         <v>80</v>
@@ -4775,13 +4785,13 @@
         <v>44964</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="J18" s="24" t="s">
         <v>80</v>
@@ -4798,7 +4808,7 @@
         <v>80</v>
       </c>
       <c r="P18" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q18" s="24"/>
       <c r="R18" s="25"/>
@@ -4827,13 +4837,13 @@
         <v>44964</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="J19" s="24" t="s">
         <v>80</v>
@@ -4850,7 +4860,7 @@
         <v>80</v>
       </c>
       <c r="P19" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q19" s="24"/>
       <c r="R19" s="25"/>
@@ -4879,13 +4889,13 @@
         <v>44964</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="J20" s="24" t="s">
         <v>80</v>
@@ -4902,7 +4912,7 @@
         <v>80</v>
       </c>
       <c r="P20" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q20" s="24"/>
       <c r="R20" s="25"/>
@@ -4931,13 +4941,13 @@
         <v>44964</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="J21" s="24" t="s">
         <v>80</v>
@@ -4954,7 +4964,7 @@
         <v>80</v>
       </c>
       <c r="P21" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q21" s="24"/>
       <c r="R21" s="25"/>
@@ -4992,7 +5002,7 @@
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="24" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="Q22" s="24"/>
       <c r="R22" s="25" t="s">
@@ -5032,7 +5042,7 @@
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
       <c r="P23" s="24" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="Q23" s="24"/>
       <c r="R23" s="25" t="s">
@@ -5063,13 +5073,13 @@
         <v>44964</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="J24" s="24" t="s">
         <v>80</v>
@@ -5086,7 +5096,7 @@
         <v>80</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="25"/>
@@ -5119,7 +5129,7 @@
         <v>191</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -5157,7 +5167,7 @@
         <v>191</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
@@ -5195,7 +5205,7 @@
         <v>191</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
@@ -5233,7 +5243,7 @@
         <v>191</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
@@ -5271,7 +5281,7 @@
         <v>191</v>
       </c>
       <c r="K29" s="24" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
@@ -5309,7 +5319,7 @@
         <v>191</v>
       </c>
       <c r="K30" s="26" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
@@ -5347,7 +5357,7 @@
         <v>191</v>
       </c>
       <c r="K31" s="24" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
@@ -5381,13 +5391,13 @@
         <v>44964</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="H32" s="23" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="J32" s="24" t="s">
         <v>80</v>
@@ -5404,7 +5414,7 @@
         <v>80</v>
       </c>
       <c r="P32" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q32" s="24"/>
       <c r="R32" s="25"/>
@@ -5433,13 +5443,13 @@
         <v>44964</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="H33" s="23" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="J33" s="24" t="s">
         <v>80</v>
@@ -5456,7 +5466,7 @@
         <v>80</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q33" s="24"/>
       <c r="R33" s="25"/>
@@ -5485,13 +5495,13 @@
         <v>44964</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="J34" s="24" t="s">
         <v>80</v>
@@ -5508,7 +5518,7 @@
         <v>80</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q34" s="24"/>
       <c r="R34" s="25"/>
@@ -5541,7 +5551,7 @@
         <v>191</v>
       </c>
       <c r="K35" s="24" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
@@ -5579,7 +5589,7 @@
         <v>191</v>
       </c>
       <c r="K36" s="24" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="L36" s="24"/>
       <c r="M36" s="24"/>
@@ -5613,13 +5623,13 @@
         <v>44960</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="H37" s="23" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="J37" s="24" t="s">
         <v>80</v>
@@ -5636,7 +5646,7 @@
         <v>80</v>
       </c>
       <c r="P37" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q37" s="24"/>
       <c r="R37" s="25"/>
@@ -5669,7 +5679,7 @@
         <v>191</v>
       </c>
       <c r="K38" s="24" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="L38" s="24"/>
       <c r="M38" s="24"/>
@@ -5707,7 +5717,7 @@
         <v>191</v>
       </c>
       <c r="K39" s="24" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="L39" s="24"/>
       <c r="M39" s="24"/>
@@ -5745,7 +5755,7 @@
         <v>191</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
@@ -5783,7 +5793,7 @@
         <v>191</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="L41" s="24"/>
       <c r="M41" s="24"/>
@@ -5821,7 +5831,7 @@
         <v>191</v>
       </c>
       <c r="K42" s="24" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
@@ -5859,7 +5869,7 @@
         <v>191</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
@@ -5897,7 +5907,7 @@
         <v>191</v>
       </c>
       <c r="K44" s="24" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
@@ -5935,7 +5945,7 @@
         <v>191</v>
       </c>
       <c r="K45" s="24" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
@@ -5973,7 +5983,7 @@
         <v>191</v>
       </c>
       <c r="K46" s="24" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
@@ -6007,13 +6017,13 @@
         <v>44960</v>
       </c>
       <c r="G47" s="23" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="J47" s="24" t="s">
         <v>80</v>
@@ -6030,7 +6040,7 @@
         <v>80</v>
       </c>
       <c r="P47" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q47" s="24"/>
       <c r="R47" s="25"/>
@@ -6059,13 +6069,13 @@
         <v>44963</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="J48" s="24" t="s">
         <v>80</v>
@@ -6082,7 +6092,7 @@
         <v>80</v>
       </c>
       <c r="P48" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q48" s="24"/>
       <c r="R48" s="25"/>
@@ -6115,7 +6125,7 @@
         <v>191</v>
       </c>
       <c r="K49" s="24" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
@@ -6153,7 +6163,7 @@
         <v>191</v>
       </c>
       <c r="K50" s="24" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
@@ -6187,13 +6197,13 @@
         <v>44971</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="H51" s="23" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="J51" s="24" t="s">
         <v>80</v>
@@ -6210,7 +6220,7 @@
         <v>80</v>
       </c>
       <c r="P51" s="24" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="Q51" s="24"/>
       <c r="R51" s="25"/>
@@ -15831,8 +15841,8 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Nuovo commit file errors.json del 9/05/2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
@@ -291,13 +291,13 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:02:23Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0698a6ab1c2b267b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.e6d79519fedee7ac950f4a87d2aec34f6a0cf56aa1aff9f14d900e83358db4da.bb2c54364e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:08:42Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91db63643e5c59bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.a6ef72b27e3e24be5488e2e1e2a56be7066adb5afbe1e2cfcbb99b599ef802ab.f16bb04fd0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -314,13 +314,13 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:08:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12cd0759a89e8bc0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.6c94985af013618bf88b3847bd6ab478cbbf15f8f4fede722997d6c474425a6b.5d3f4e032a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:10:02Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d01a1893dfacd6a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.f0a0e2fdbbc0508c28558f8d752b3fd271684cba94e5260e46b0710f68fe7dad.5897b0aa7d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_CERT_VAC_CT3</t>
@@ -331,13 +331,13 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:11:56Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e1aea4b961b59d70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.286b0d0b47d90092ddd09b37f0b9cf1ca319e1eb12ceea5c0c5a222bc2eb8312.46ff662d1c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:19:35Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d514450e65e94261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.35ff41ca069695bd56d41cd755accbecbb4b49e2321f4eae26fb77849adf8512.cba403900d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_CERT_VAC_CT4</t>
@@ -348,13 +348,13 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:13:30Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8c67a41708088f2f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.bfd7a292c5febec7be955e34f5ee401cde3ab135ebc2048c099fddc620bca876.ba02251863^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:22:52Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1836dc5d370a2f9e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.073e033d5a2095124a3f32d5039b980dbc3222910eaaaac258f80740cdf7e058.f10eeb4fe3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SING_VAC</t>
@@ -368,13 +368,13 @@
 Il Documento CDA2 Scheda Singola Vaccinazione dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:15:05Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102fdd72ff5ef74c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.e554f3d962432ad420cab71c8d58f4422835e978faf2617d4bbe60ed2559ed29.e69455db6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:24:10Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1e7a477544d74d23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.6754b85cf72dcc748fe53fc78fa14cdf1842eebd9a8dad1f3636b0a264fb5338.64cd34192e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_SING_VAC_CT2</t>
@@ -385,13 +385,13 @@
 Il Documento CDA2 Scheda Singola Vaccinazione dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:17:54Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">208f654192a0a354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.a018865dde3d6596cc57e8d4c46afbdb6ab12f4b2521f6477eef002b1b4950b3.2410fb72e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:25:32Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80c68c048cf6a3db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.98711e0d3af60d2e89180c57135e600313a70aa0df7c47c83635ceaeef487391.9dd85fe3e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_SING_VAC_CT3</t>
@@ -402,13 +402,13 @@
 Il Documento CDA2 Scheda Singola Vaccinazione dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti"casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:20:03Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">825685cf224e2dd9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.69116858ea2f194d9b36afd7ef73c8a23c4c9e19034fbea0e807108c2ae3a9d8.b3426ebf87^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:27:48Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155141ca865ed022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.0219d21279372c58c45dc853c70c535a3ed04843cea7808bf333a687365cf423.b66e1b55fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_SING_VAC_CT4</t>
@@ -419,13 +419,13 @@
 Il Documento CDA2 Scheda Singola Vaccinazione dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-09T09:21:56Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dbdd7864c8863333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.e854535ecf8baf7eb1c9c19fe21a87da40cd70cdfbb4717c36b8c3753c186d21.26da7903cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-10T17:28:58Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9033cb35de4ee319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.9ef9583c67c8a2ce180240fda4185fa0c3dda70804cd783737608712a5e28ac9.a0d384a334^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CERT_VAC_KO</t>
@@ -1091,7 +1091,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1159,12 +1159,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -1308,13 +1302,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1361,12 +1359,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1381,14 +1375,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -1397,12 +1383,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1442,11 +1436,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1465,24 +1455,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1642,67 +1624,67 @@
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="130.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="2" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="191.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2715,99 +2697,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="3.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="194.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="2" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="A6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
+      <c r="A8" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="n">
+      <c r="A9" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="n">
+      <c r="A10" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
+      <c r="A11" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+      <c r="A12" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="n">
+      <c r="A13" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3815,33 +3797,33 @@
   <dimension ref="A1:T669"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="13" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="14" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="21" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="46.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="63.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="104.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="14" width="33.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="2" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="33.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="21" style="2" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1" s="5"/>
+      <c r="C1" s="6"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -3855,12 +3837,12 @@
       <c r="P1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3873,18 +3855,18 @@
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="3"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="22"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -3897,17 +3879,17 @@
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="3"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="5"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -3920,17 +3902,17 @@
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="19"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="22"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -3943,8 +3925,8 @@
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="3"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="24"/>
@@ -3962,7 +3944,7 @@
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
-      <c r="R6" s="18"/>
+      <c r="R6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="25"/>
@@ -3980,7 +3962,7 @@
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
-      <c r="R7" s="18"/>
+      <c r="R7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F8" s="15"/>
@@ -4073,7 +4055,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="32" t="n">
-        <v>45055</v>
+        <v>45056</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>51</v>
@@ -4081,22 +4063,22 @@
       <c r="H10" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="38" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="37" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4117,7 +4099,7 @@
         <v>57</v>
       </c>
       <c r="F11" s="32" t="n">
-        <v>45055</v>
+        <v>45056</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>58</v>
@@ -4125,22 +4107,22 @@
       <c r="H11" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="39" t="s">
+      <c r="I11" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="38" t="s">
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="37" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4161,7 +4143,7 @@
         <v>62</v>
       </c>
       <c r="F12" s="32" t="n">
-        <v>45055</v>
+        <v>45056</v>
       </c>
       <c r="G12" s="33" t="s">
         <v>63</v>
@@ -4169,22 +4151,22 @@
       <c r="H12" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="38" t="s">
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="37" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4204,31 +4186,31 @@
       <c r="E13" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="40" t="n">
-        <v>45055</v>
-      </c>
-      <c r="G13" s="41" t="s">
+      <c r="F13" s="32" t="n">
+        <v>45056</v>
+      </c>
+      <c r="G13" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="J13" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="38" t="s">
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="37" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4248,31 +4230,31 @@
       <c r="E14" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="40" t="n">
-        <v>45055</v>
-      </c>
-      <c r="G14" s="41" t="s">
+      <c r="F14" s="32" t="n">
+        <v>45056</v>
+      </c>
+      <c r="G14" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="35" t="s">
+      <c r="J14" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="38" t="s">
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="37" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4292,35 +4274,35 @@
       <c r="E15" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="40" t="n">
-        <v>45055</v>
-      </c>
-      <c r="G15" s="41" t="s">
+      <c r="F15" s="32" t="n">
+        <v>45056</v>
+      </c>
+      <c r="G15" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="J15" s="35" t="s">
+      <c r="J15" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="38" t="s">
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="n">
         <v>22</v>
       </c>
@@ -4336,35 +4318,35 @@
       <c r="E16" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="40" t="n">
-        <v>45055</v>
-      </c>
-      <c r="G16" s="41" t="s">
+      <c r="F16" s="32" t="n">
+        <v>45056</v>
+      </c>
+      <c r="G16" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="41" t="s">
+      <c r="I16" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="38" t="s">
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="n">
         <v>23</v>
       </c>
@@ -4380,31 +4362,31 @@
       <c r="E17" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="40" t="n">
-        <v>45055</v>
-      </c>
-      <c r="G17" s="41" t="s">
+      <c r="F17" s="32" t="n">
+        <v>45056</v>
+      </c>
+      <c r="G17" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="42" t="s">
+      <c r="I17" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="J17" s="35" t="s">
+      <c r="J17" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="38" t="s">
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="37" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4421,7 +4403,7 @@
       <c r="D18" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="39" t="s">
         <v>93</v>
       </c>
       <c r="F18" s="40" t="n">
@@ -4436,27 +4418,27 @@
       <c r="I18" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35" t="s">
+      <c r="K18" s="34"/>
+      <c r="L18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35" t="s">
+      <c r="N18" s="34"/>
+      <c r="O18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P18" s="35" t="s">
+      <c r="P18" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="38" t="s">
+      <c r="Q18" s="34"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4473,42 +4455,42 @@
       <c r="D19" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="39" t="s">
         <v>93</v>
       </c>
       <c r="F19" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I19" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35" t="s">
+      <c r="K19" s="34"/>
+      <c r="L19" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="35" t="s">
+      <c r="M19" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35" t="s">
+      <c r="N19" s="34"/>
+      <c r="O19" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P19" s="35" t="s">
+      <c r="P19" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="38" t="s">
+      <c r="Q19" s="34"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4525,42 +4507,42 @@
       <c r="D20" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="39" t="s">
         <v>105</v>
       </c>
       <c r="F20" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="H20" s="44" t="s">
+      <c r="H20" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35" t="s">
+      <c r="K20" s="34"/>
+      <c r="L20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="35" t="s">
+      <c r="M20" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35" t="s">
+      <c r="N20" s="34"/>
+      <c r="O20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P20" s="35" t="s">
+      <c r="P20" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="38" t="s">
+      <c r="Q20" s="34"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4577,42 +4559,42 @@
       <c r="D21" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="39" t="s">
         <v>105</v>
       </c>
       <c r="F21" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35" t="s">
+      <c r="K21" s="34"/>
+      <c r="L21" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M21" s="35" t="s">
+      <c r="M21" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35" t="s">
+      <c r="N21" s="34"/>
+      <c r="O21" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P21" s="35" t="s">
+      <c r="P21" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="38" t="s">
+      <c r="Q21" s="34"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4633,26 +4615,26 @@
         <v>113</v>
       </c>
       <c r="F22" s="32"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="35" t="s">
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35" t="s">
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="36" t="s">
+      <c r="Q22" s="34"/>
+      <c r="R22" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="S22" s="37"/>
-      <c r="T22" s="38" t="s">
+      <c r="S22" s="36"/>
+      <c r="T22" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4673,26 +4655,26 @@
         <v>113</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="35" t="s">
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35" t="s">
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="36" t="s">
+      <c r="Q23" s="34"/>
+      <c r="R23" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="S23" s="37"/>
-      <c r="T23" s="38" t="s">
+      <c r="S23" s="36"/>
+      <c r="T23" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4715,36 +4697,36 @@
       <c r="F24" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G24" s="44" t="s">
+      <c r="G24" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="H24" s="44" t="s">
+      <c r="H24" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="J24" s="35" t="s">
+      <c r="J24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35" t="s">
+      <c r="K24" s="34"/>
+      <c r="L24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="35" t="s">
+      <c r="M24" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35" t="s">
+      <c r="N24" s="34"/>
+      <c r="O24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P24" s="35" t="s">
+      <c r="P24" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="38" t="s">
+      <c r="Q24" s="34"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4765,24 +4747,24 @@
         <v>119</v>
       </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="35" t="s">
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K25" s="35" t="s">
+      <c r="K25" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="38" t="s">
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4803,24 +4785,24 @@
         <v>122</v>
       </c>
       <c r="F26" s="32"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="35" t="s">
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K26" s="35" t="s">
+      <c r="K26" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="37"/>
-      <c r="T26" s="38" t="s">
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4841,24 +4823,24 @@
         <v>125</v>
       </c>
       <c r="F27" s="32"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="35" t="s">
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K27" s="35" t="s">
+      <c r="K27" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="38" t="s">
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4879,24 +4861,24 @@
         <v>128</v>
       </c>
       <c r="F28" s="32"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="35" t="s">
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K28" s="35" t="s">
+      <c r="K28" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="38" t="s">
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4917,24 +4899,24 @@
         <v>131</v>
       </c>
       <c r="F29" s="32"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="35" t="s">
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K29" s="35" t="s">
+      <c r="K29" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="38" t="s">
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4955,24 +4937,24 @@
         <v>134</v>
       </c>
       <c r="F30" s="32"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="35" t="s">
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K30" s="37" t="s">
+      <c r="K30" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="37"/>
-      <c r="T30" s="38" t="s">
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4993,24 +4975,24 @@
         <v>137</v>
       </c>
       <c r="F31" s="32"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="35" t="s">
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K31" s="35" t="s">
+      <c r="K31" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="38" t="s">
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="34"/>
+      <c r="Q31" s="34"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5033,36 +5015,36 @@
       <c r="F32" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G32" s="44" t="s">
+      <c r="G32" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="44" t="s">
+      <c r="H32" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="I32" s="44" t="s">
+      <c r="I32" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="J32" s="35" t="s">
+      <c r="J32" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35" t="s">
+      <c r="K32" s="34"/>
+      <c r="L32" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M32" s="35" t="s">
+      <c r="M32" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35" t="s">
+      <c r="N32" s="34"/>
+      <c r="O32" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P32" s="35" t="s">
+      <c r="P32" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="38" t="s">
+      <c r="Q32" s="34"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5085,36 +5067,36 @@
       <c r="F33" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G33" s="44" t="s">
+      <c r="G33" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="H33" s="44" t="s">
+      <c r="H33" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="I33" s="44" t="s">
+      <c r="I33" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="J33" s="35" t="s">
+      <c r="J33" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35" t="s">
+      <c r="K33" s="34"/>
+      <c r="L33" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M33" s="35" t="s">
+      <c r="M33" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N33" s="35"/>
-      <c r="O33" s="35" t="s">
+      <c r="N33" s="34"/>
+      <c r="O33" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P33" s="35" t="s">
+      <c r="P33" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="38" t="s">
+      <c r="Q33" s="34"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5137,36 +5119,36 @@
       <c r="F34" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G34" s="44" t="s">
+      <c r="G34" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="44" t="s">
+      <c r="H34" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="I34" s="44" t="s">
+      <c r="I34" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="J34" s="35" t="s">
+      <c r="J34" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35" t="s">
+      <c r="K34" s="34"/>
+      <c r="L34" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M34" s="35" t="s">
+      <c r="M34" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35" t="s">
+      <c r="N34" s="34"/>
+      <c r="O34" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P34" s="35" t="s">
+      <c r="P34" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="38" t="s">
+      <c r="Q34" s="34"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="36"/>
+      <c r="T34" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5187,24 +5169,24 @@
         <v>155</v>
       </c>
       <c r="F35" s="32"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="35" t="s">
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K35" s="35" t="s">
+      <c r="K35" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="36"/>
-      <c r="S35" s="37"/>
-      <c r="T35" s="38" t="s">
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34"/>
+      <c r="P35" s="34"/>
+      <c r="Q35" s="34"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="36"/>
+      <c r="T35" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5225,24 +5207,24 @@
         <v>157</v>
       </c>
       <c r="F36" s="32"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="35" t="s">
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K36" s="35" t="s">
+      <c r="K36" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="37"/>
-      <c r="T36" s="38" t="s">
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5265,36 +5247,36 @@
       <c r="F37" s="32" t="n">
         <v>44960</v>
       </c>
-      <c r="G37" s="44" t="s">
+      <c r="G37" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="H37" s="44" t="s">
+      <c r="H37" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="J37" s="35" t="s">
+      <c r="J37" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35" t="s">
+      <c r="K37" s="34"/>
+      <c r="L37" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M37" s="35" t="s">
+      <c r="M37" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N37" s="35"/>
-      <c r="O37" s="35" t="s">
+      <c r="N37" s="34"/>
+      <c r="O37" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P37" s="35" t="s">
+      <c r="P37" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q37" s="35"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="38" t="s">
+      <c r="Q37" s="34"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="36"/>
+      <c r="T37" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5315,24 +5297,24 @@
         <v>164</v>
       </c>
       <c r="F38" s="32"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="35" t="s">
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K38" s="35" t="s">
+      <c r="K38" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="37"/>
-      <c r="T38" s="38" t="s">
+      <c r="L38" s="34"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="34"/>
+      <c r="P38" s="34"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="36"/>
+      <c r="T38" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5353,24 +5335,24 @@
         <v>167</v>
       </c>
       <c r="F39" s="32"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="35" t="s">
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K39" s="35" t="s">
+      <c r="K39" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="37"/>
-      <c r="T39" s="38" t="s">
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="35"/>
+      <c r="S39" s="36"/>
+      <c r="T39" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5391,24 +5373,24 @@
         <v>169</v>
       </c>
       <c r="F40" s="32"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="35" t="s">
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K40" s="35" t="s">
+      <c r="K40" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="38" t="s">
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
+      <c r="P40" s="34"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="36"/>
+      <c r="T40" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5429,24 +5411,24 @@
         <v>171</v>
       </c>
       <c r="F41" s="32"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="35" t="s">
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K41" s="35" t="s">
+      <c r="K41" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="36"/>
-      <c r="S41" s="37"/>
-      <c r="T41" s="38" t="s">
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="34"/>
+      <c r="P41" s="34"/>
+      <c r="Q41" s="34"/>
+      <c r="R41" s="35"/>
+      <c r="S41" s="36"/>
+      <c r="T41" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5467,24 +5449,24 @@
         <v>173</v>
       </c>
       <c r="F42" s="32"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="35" t="s">
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K42" s="35" t="s">
+      <c r="K42" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="36"/>
-      <c r="S42" s="37"/>
-      <c r="T42" s="38" t="s">
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
+      <c r="P42" s="34"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="36"/>
+      <c r="T42" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5505,24 +5487,24 @@
         <v>175</v>
       </c>
       <c r="F43" s="32"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="35" t="s">
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K43" s="35" t="s">
+      <c r="K43" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="36"/>
-      <c r="S43" s="37"/>
-      <c r="T43" s="38" t="s">
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
+      <c r="P43" s="34"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="36"/>
+      <c r="T43" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5543,24 +5525,24 @@
         <v>177</v>
       </c>
       <c r="F44" s="32"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="35" t="s">
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K44" s="35" t="s">
+      <c r="K44" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="35"/>
-      <c r="P44" s="35"/>
-      <c r="Q44" s="35"/>
-      <c r="R44" s="36"/>
-      <c r="S44" s="37"/>
-      <c r="T44" s="38" t="s">
+      <c r="L44" s="34"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="34"/>
+      <c r="O44" s="34"/>
+      <c r="P44" s="34"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="35"/>
+      <c r="S44" s="36"/>
+      <c r="T44" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5581,24 +5563,24 @@
         <v>180</v>
       </c>
       <c r="F45" s="32"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="35" t="s">
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K45" s="35" t="s">
+      <c r="K45" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-      <c r="O45" s="35"/>
-      <c r="P45" s="35"/>
-      <c r="Q45" s="35"/>
-      <c r="R45" s="36"/>
-      <c r="S45" s="37"/>
-      <c r="T45" s="38" t="s">
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="34"/>
+      <c r="P45" s="34"/>
+      <c r="Q45" s="34"/>
+      <c r="R45" s="35"/>
+      <c r="S45" s="36"/>
+      <c r="T45" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5619,24 +5601,24 @@
         <v>183</v>
       </c>
       <c r="F46" s="32"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="35" t="s">
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K46" s="35" t="s">
+      <c r="K46" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="36"/>
-      <c r="S46" s="37"/>
-      <c r="T46" s="38" t="s">
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
+      <c r="P46" s="34"/>
+      <c r="Q46" s="34"/>
+      <c r="R46" s="35"/>
+      <c r="S46" s="36"/>
+      <c r="T46" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5659,36 +5641,36 @@
       <c r="F47" s="32" t="n">
         <v>44960</v>
       </c>
-      <c r="G47" s="44" t="s">
+      <c r="G47" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="H47" s="44" t="s">
+      <c r="H47" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="I47" s="44" t="s">
+      <c r="I47" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="J47" s="35" t="s">
+      <c r="J47" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K47" s="35"/>
-      <c r="L47" s="35" t="s">
+      <c r="K47" s="34"/>
+      <c r="L47" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M47" s="35" t="s">
+      <c r="M47" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N47" s="35"/>
-      <c r="O47" s="35" t="s">
+      <c r="N47" s="34"/>
+      <c r="O47" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P47" s="35" t="s">
+      <c r="P47" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q47" s="35"/>
-      <c r="R47" s="36"/>
-      <c r="S47" s="37"/>
-      <c r="T47" s="38" t="s">
+      <c r="Q47" s="34"/>
+      <c r="R47" s="35"/>
+      <c r="S47" s="36"/>
+      <c r="T47" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5711,36 +5693,36 @@
       <c r="F48" s="32" t="n">
         <v>44963</v>
       </c>
-      <c r="G48" s="44" t="s">
+      <c r="G48" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="H48" s="44" t="s">
+      <c r="H48" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="I48" s="44" t="s">
+      <c r="I48" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="J48" s="35" t="s">
+      <c r="J48" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35" t="s">
+      <c r="K48" s="34"/>
+      <c r="L48" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M48" s="35" t="s">
+      <c r="M48" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N48" s="35"/>
-      <c r="O48" s="35" t="s">
+      <c r="N48" s="34"/>
+      <c r="O48" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P48" s="35" t="s">
+      <c r="P48" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q48" s="35"/>
-      <c r="R48" s="36"/>
-      <c r="S48" s="37"/>
-      <c r="T48" s="38" t="s">
+      <c r="Q48" s="34"/>
+      <c r="R48" s="35"/>
+      <c r="S48" s="36"/>
+      <c r="T48" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5761,24 +5743,24 @@
         <v>195</v>
       </c>
       <c r="F49" s="32"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="35" t="s">
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K49" s="35" t="s">
+      <c r="K49" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="35"/>
-      <c r="P49" s="35"/>
-      <c r="Q49" s="35"/>
-      <c r="R49" s="36"/>
-      <c r="S49" s="37"/>
-      <c r="T49" s="38" t="s">
+      <c r="L49" s="34"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="34"/>
+      <c r="O49" s="34"/>
+      <c r="P49" s="34"/>
+      <c r="Q49" s="34"/>
+      <c r="R49" s="35"/>
+      <c r="S49" s="36"/>
+      <c r="T49" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5799,24 +5781,24 @@
         <v>197</v>
       </c>
       <c r="F50" s="32"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="35" t="s">
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K50" s="35" t="s">
+      <c r="K50" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
-      <c r="N50" s="35"/>
-      <c r="O50" s="35"/>
-      <c r="P50" s="35"/>
-      <c r="Q50" s="35"/>
-      <c r="R50" s="36"/>
-      <c r="S50" s="37"/>
-      <c r="T50" s="38" t="s">
+      <c r="L50" s="34"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="34"/>
+      <c r="O50" s="34"/>
+      <c r="P50" s="34"/>
+      <c r="Q50" s="34"/>
+      <c r="R50" s="35"/>
+      <c r="S50" s="36"/>
+      <c r="T50" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5839,36 +5821,36 @@
       <c r="F51" s="32" t="n">
         <v>44971</v>
       </c>
-      <c r="G51" s="44" t="s">
+      <c r="G51" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="H51" s="44" t="s">
+      <c r="H51" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="I51" s="44" t="s">
+      <c r="I51" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="J51" s="35" t="s">
+      <c r="J51" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35" t="s">
+      <c r="K51" s="34"/>
+      <c r="L51" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M51" s="35" t="s">
+      <c r="M51" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N51" s="35"/>
-      <c r="O51" s="35" t="s">
+      <c r="N51" s="34"/>
+      <c r="O51" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P51" s="35" t="s">
+      <c r="P51" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="Q51" s="35"/>
-      <c r="R51" s="36"/>
-      <c r="S51" s="37"/>
-      <c r="T51" s="38" t="s">
+      <c r="Q51" s="34"/>
+      <c r="R51" s="35"/>
+      <c r="S51" s="36"/>
+      <c r="T51" s="37" t="s">
         <v>99</v>
       </c>
     </row>
@@ -12625,712 +12607,712 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="102"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="2" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="42" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="43" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="42" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="43" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="43" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="43" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="43" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="45" t="n">
+      <c r="C10" s="42" t="n">
         <v>191</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="42" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C11" s="45" t="n">
+      <c r="C11" s="42" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="42" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C12" s="45" t="n">
+      <c r="C12" s="42" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="42" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="45" t="n">
+      <c r="C13" s="42" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="43" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C14" s="45" t="n">
+      <c r="C14" s="42" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="42" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C15" s="45" t="n">
+      <c r="C15" s="42" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="43" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C16" s="45" t="n">
+      <c r="C16" s="42" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="43" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="45" t="n">
+      <c r="C17" s="42" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="43" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C18" s="45" t="n">
+      <c r="C18" s="42" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="43" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C19" s="45" t="n">
+      <c r="C19" s="42" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="42" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C20" s="45" t="n">
+      <c r="C20" s="42" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="42" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C21" s="45" t="n">
+      <c r="C21" s="42" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="43" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C22" s="45" t="n">
+      <c r="C22" s="42" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="42" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C23" s="45" t="n">
+      <c r="C23" s="42" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="43" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C24" s="45" t="n">
+      <c r="C24" s="42" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="43" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C25" s="45" t="n">
+      <c r="C25" s="42" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="43" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C26" s="45" t="n">
+      <c r="C26" s="42" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="43" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="45" t="n">
+      <c r="C27" s="42" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="42" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C28" s="45" t="n">
+      <c r="C28" s="42" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="42" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C29" s="45" t="n">
+      <c r="C29" s="42" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="44" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="45" t="n">
+      <c r="C30" s="42" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="42" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C31" s="45" t="n">
+      <c r="C31" s="42" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="43" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C32" s="45" t="n">
+      <c r="C32" s="42" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="43" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C33" s="45" t="n">
+      <c r="C33" s="42" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="43" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C34" s="45" t="n">
+      <c r="C34" s="42" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="43" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C35" s="45" t="n">
+      <c r="C35" s="42" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="45" t="n">
+      <c r="D35" s="42" t="n">
         <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C36" s="45" t="n">
+      <c r="C36" s="42" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="45" t="n">
+      <c r="D36" s="42" t="n">
         <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C37" s="45" t="n">
+      <c r="C37" s="42" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="46" t="n">
+      <c r="D37" s="43" t="n">
         <v>236</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C38" s="45" t="n">
+      <c r="C38" s="42" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="45" t="n">
+      <c r="D38" s="42" t="n">
         <v>252</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C39" s="45" t="n">
+      <c r="C39" s="42" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="46" t="n">
+      <c r="D39" s="43" t="n">
         <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C40" s="45" t="n">
+      <c r="C40" s="42" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="46" t="n">
+      <c r="D40" s="43" t="n">
         <v>284</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C41" s="45" t="n">
+      <c r="C41" s="42" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="46" t="n">
+      <c r="D41" s="43" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C42" s="45" t="n">
+      <c r="C42" s="42" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="46" t="n">
+      <c r="D42" s="43" t="n">
         <v>316</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C43" s="45" t="n">
+      <c r="C43" s="42" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="45" t="n">
+      <c r="D43" s="42" t="n">
         <v>207</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C44" s="45" t="n">
+      <c r="C44" s="42" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="45" t="n">
+      <c r="D44" s="42" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C45" s="45" t="n">
+      <c r="C45" s="42" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="46" t="n">
+      <c r="D45" s="43" t="n">
         <v>239</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C46" s="45" t="n">
+      <c r="C46" s="42" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="45" t="n">
+      <c r="D46" s="42" t="n">
         <v>255</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C47" s="45" t="n">
+      <c r="C47" s="42" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="46" t="n">
+      <c r="D47" s="43" t="n">
         <v>271</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C48" s="45" t="n">
+      <c r="C48" s="42" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="46" t="n">
+      <c r="D48" s="43" t="n">
         <v>287</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C49" s="45" t="n">
+      <c r="C49" s="42" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="46" t="n">
+      <c r="D49" s="43" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C50" s="45" t="n">
+      <c r="C50" s="42" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="46" t="n">
+      <c r="D50" s="43" t="n">
         <v>319</v>
       </c>
     </row>
@@ -14305,38 +14287,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="2" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="45" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="45" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Corretti test ID [34, 16, 42] come richiesto nella mail dell' 11/05
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
@@ -291,13 +291,13 @@
 Il Documento CDA2 Certificato Vaccinale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-10T17:08:42Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91db63643e5c59bd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.a6ef72b27e3e24be5488e2e1e2a56be7066adb5afbe1e2cfcbb99b599ef802ab.f16bb04fd0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-05-12T10:50:54Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b6874f0a8887f6c1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.02cba4da6fdf728f34c2c39dad5fdf1ffcdaca5f44c9565e0b25d88ca8952303.6ddaaf271d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -502,10 +502,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_SING_VAC_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-07T15:15:43Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a572041ef60ffa35</t>
+    <t xml:space="preserve">2023-05-12T09:45:30Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8a6a374cbb158aa0</t>
   </si>
   <si>
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
@@ -576,10 +576,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_SING_VAC_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-07T15:21:32Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d1852c8b8d83fbf3</t>
+    <t xml:space="preserve">2023-05-12T09:47:15Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fb126ea724b5755f</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CERT_VAC_TIMEOUT</t>
@@ -1302,7 +1302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1455,7 +1455,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1617,8 +1621,8 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="F10:I10 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2691,8 +2695,8 @@
   </sheetPr>
   <dimension ref="A1:B998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:I10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3796,12 +3800,12 @@
   </sheetPr>
   <dimension ref="A1:T669"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="I10" activeCellId="0" sqref="F10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4038,7 +4042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="n">
         <v>16</v>
       </c>
@@ -4055,7 +4059,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="32" t="n">
-        <v>45056</v>
+        <v>45058</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>51</v>
@@ -4101,13 +4105,13 @@
       <c r="F11" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="38" t="s">
         <v>60</v>
       </c>
       <c r="J11" s="34" t="s">
@@ -4145,13 +4149,13 @@
       <c r="F12" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="38" t="s">
         <v>65</v>
       </c>
       <c r="J12" s="34" t="s">
@@ -4189,13 +4193,13 @@
       <c r="F13" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="38" t="s">
         <v>70</v>
       </c>
       <c r="J13" s="34" t="s">
@@ -4233,13 +4237,13 @@
       <c r="F14" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="I14" s="38" t="s">
         <v>76</v>
       </c>
       <c r="J14" s="34" t="s">
@@ -4277,13 +4281,13 @@
       <c r="F15" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="38" t="s">
         <v>81</v>
       </c>
       <c r="J15" s="34" t="s">
@@ -4321,13 +4325,13 @@
       <c r="F16" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="39" t="s">
         <v>86</v>
       </c>
       <c r="J16" s="34" t="s">
@@ -4365,13 +4369,13 @@
       <c r="F17" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="39" t="s">
         <v>91</v>
       </c>
       <c r="J17" s="34" t="s">
@@ -4403,19 +4407,19 @@
       <c r="D18" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="40" t="n">
+      <c r="F18" s="41" t="n">
         <v>44964</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="40" t="s">
+      <c r="H18" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="41" t="s">
         <v>96</v>
       </c>
       <c r="J18" s="34" t="s">
@@ -4442,7 +4446,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="n">
         <v>34</v>
       </c>
@@ -4455,19 +4459,19 @@
       <c r="D19" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="40" t="s">
         <v>93</v>
       </c>
       <c r="F19" s="32" t="n">
-        <v>44964</v>
-      </c>
-      <c r="G19" s="41" t="s">
+        <v>45058</v>
+      </c>
+      <c r="G19" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="41" t="s">
+      <c r="I19" s="33" t="s">
         <v>103</v>
       </c>
       <c r="J19" s="34" t="s">
@@ -4507,19 +4511,19 @@
       <c r="D20" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="40" t="s">
         <v>105</v>
       </c>
       <c r="F20" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="41" t="s">
+      <c r="I20" s="42" t="s">
         <v>108</v>
       </c>
       <c r="J20" s="34" t="s">
@@ -4546,7 +4550,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="29" t="n">
         <v>42</v>
       </c>
@@ -4559,19 +4563,19 @@
       <c r="D21" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="40" t="s">
         <v>105</v>
       </c>
       <c r="F21" s="32" t="n">
-        <v>44964</v>
-      </c>
-      <c r="G21" s="41" t="s">
+        <v>45058</v>
+      </c>
+      <c r="G21" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="41" t="s">
+      <c r="H21" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="33" t="s">
         <v>103</v>
       </c>
       <c r="J21" s="34" t="s">
@@ -4615,9 +4619,9 @@
         <v>113</v>
       </c>
       <c r="F22" s="32"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="34" t="s">
         <v>54</v>
       </c>
@@ -4655,9 +4659,9 @@
         <v>113</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
       <c r="J23" s="34" t="s">
         <v>54</v>
       </c>
@@ -4697,13 +4701,13 @@
       <c r="F24" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="42" t="s">
         <v>96</v>
       </c>
       <c r="J24" s="34" t="s">
@@ -4747,9 +4751,9 @@
         <v>119</v>
       </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
       <c r="J25" s="34" t="s">
         <v>97</v>
       </c>
@@ -4785,9 +4789,9 @@
         <v>122</v>
       </c>
       <c r="F26" s="32"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
       <c r="J26" s="34" t="s">
         <v>97</v>
       </c>
@@ -4823,9 +4827,9 @@
         <v>125</v>
       </c>
       <c r="F27" s="32"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
       <c r="J27" s="34" t="s">
         <v>97</v>
       </c>
@@ -4861,9 +4865,9 @@
         <v>128</v>
       </c>
       <c r="F28" s="32"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
       <c r="J28" s="34" t="s">
         <v>97</v>
       </c>
@@ -4899,9 +4903,9 @@
         <v>131</v>
       </c>
       <c r="F29" s="32"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
       <c r="J29" s="34" t="s">
         <v>97</v>
       </c>
@@ -4937,9 +4941,9 @@
         <v>134</v>
       </c>
       <c r="F30" s="32"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="34" t="s">
         <v>97</v>
       </c>
@@ -4975,9 +4979,9 @@
         <v>137</v>
       </c>
       <c r="F31" s="32"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
       <c r="J31" s="34" t="s">
         <v>97</v>
       </c>
@@ -5015,13 +5019,13 @@
       <c r="F32" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G32" s="41" t="s">
+      <c r="G32" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="I32" s="41" t="s">
+      <c r="I32" s="42" t="s">
         <v>143</v>
       </c>
       <c r="J32" s="34" t="s">
@@ -5067,13 +5071,13 @@
       <c r="F33" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="I33" s="41" t="s">
+      <c r="I33" s="42" t="s">
         <v>148</v>
       </c>
       <c r="J33" s="34" t="s">
@@ -5119,13 +5123,13 @@
       <c r="F34" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G34" s="41" t="s">
+      <c r="G34" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="41" t="s">
+      <c r="H34" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="42" t="s">
         <v>153</v>
       </c>
       <c r="J34" s="34" t="s">
@@ -5169,9 +5173,9 @@
         <v>155</v>
       </c>
       <c r="F35" s="32"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
       <c r="J35" s="34" t="s">
         <v>97</v>
       </c>
@@ -5207,9 +5211,9 @@
         <v>157</v>
       </c>
       <c r="F36" s="32"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
       <c r="J36" s="34" t="s">
         <v>97</v>
       </c>
@@ -5247,13 +5251,13 @@
       <c r="F37" s="32" t="n">
         <v>44960</v>
       </c>
-      <c r="G37" s="41" t="s">
+      <c r="G37" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="H37" s="41" t="s">
+      <c r="H37" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="I37" s="41" t="s">
+      <c r="I37" s="42" t="s">
         <v>162</v>
       </c>
       <c r="J37" s="34" t="s">
@@ -5297,9 +5301,9 @@
         <v>164</v>
       </c>
       <c r="F38" s="32"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
       <c r="J38" s="34" t="s">
         <v>97</v>
       </c>
@@ -5335,9 +5339,9 @@
         <v>167</v>
       </c>
       <c r="F39" s="32"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
       <c r="J39" s="34" t="s">
         <v>97</v>
       </c>
@@ -5373,9 +5377,9 @@
         <v>169</v>
       </c>
       <c r="F40" s="32"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
       <c r="J40" s="34" t="s">
         <v>97</v>
       </c>
@@ -5411,9 +5415,9 @@
         <v>171</v>
       </c>
       <c r="F41" s="32"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
       <c r="J41" s="34" t="s">
         <v>97</v>
       </c>
@@ -5449,9 +5453,9 @@
         <v>173</v>
       </c>
       <c r="F42" s="32"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
       <c r="J42" s="34" t="s">
         <v>97</v>
       </c>
@@ -5487,9 +5491,9 @@
         <v>175</v>
       </c>
       <c r="F43" s="32"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
       <c r="J43" s="34" t="s">
         <v>97</v>
       </c>
@@ -5525,9 +5529,9 @@
         <v>177</v>
       </c>
       <c r="F44" s="32"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="34" t="s">
         <v>97</v>
       </c>
@@ -5563,9 +5567,9 @@
         <v>180</v>
       </c>
       <c r="F45" s="32"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
       <c r="J45" s="34" t="s">
         <v>97</v>
       </c>
@@ -5601,9 +5605,9 @@
         <v>183</v>
       </c>
       <c r="F46" s="32"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
       <c r="J46" s="34" t="s">
         <v>97</v>
       </c>
@@ -5641,13 +5645,13 @@
       <c r="F47" s="32" t="n">
         <v>44960</v>
       </c>
-      <c r="G47" s="41" t="s">
+      <c r="G47" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="H47" s="41" t="s">
+      <c r="H47" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="I47" s="41" t="s">
+      <c r="I47" s="42" t="s">
         <v>188</v>
       </c>
       <c r="J47" s="34" t="s">
@@ -5693,13 +5697,13 @@
       <c r="F48" s="32" t="n">
         <v>44963</v>
       </c>
-      <c r="G48" s="41" t="s">
+      <c r="G48" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="H48" s="41" t="s">
+      <c r="H48" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="I48" s="41" t="s">
+      <c r="I48" s="42" t="s">
         <v>193</v>
       </c>
       <c r="J48" s="34" t="s">
@@ -5743,9 +5747,9 @@
         <v>195</v>
       </c>
       <c r="F49" s="32"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
       <c r="J49" s="34" t="s">
         <v>97</v>
       </c>
@@ -5781,9 +5785,9 @@
         <v>197</v>
       </c>
       <c r="F50" s="32"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
       <c r="J50" s="34" t="s">
         <v>97</v>
       </c>
@@ -5821,13 +5825,13 @@
       <c r="F51" s="32" t="n">
         <v>44971</v>
       </c>
-      <c r="G51" s="41" t="s">
+      <c r="G51" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="H51" s="41" t="s">
+      <c r="H51" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="I51" s="41" t="s">
+      <c r="I51" s="42" t="s">
         <v>202</v>
       </c>
       <c r="J51" s="34" t="s">
@@ -12599,10 +12603,10 @@
   </sheetPr>
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="F10:I10 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12637,10 +12641,10 @@
       <c r="B2" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="43" t="s">
         <v>208</v>
       </c>
     </row>
@@ -12651,10 +12655,10 @@
       <c r="B3" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>211</v>
       </c>
     </row>
@@ -12665,10 +12669,10 @@
       <c r="B4" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="44" t="s">
         <v>214</v>
       </c>
     </row>
@@ -12679,10 +12683,10 @@
       <c r="B5" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="43" t="s">
         <v>216</v>
       </c>
     </row>
@@ -12693,10 +12697,10 @@
       <c r="B6" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="44" t="s">
         <v>218</v>
       </c>
     </row>
@@ -12707,10 +12711,10 @@
       <c r="B7" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="44" t="s">
         <v>221</v>
       </c>
     </row>
@@ -12721,10 +12725,10 @@
       <c r="B8" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="44" t="s">
         <v>224</v>
       </c>
     </row>
@@ -12735,10 +12739,10 @@
       <c r="B9" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="44" t="s">
         <v>227</v>
       </c>
     </row>
@@ -12749,10 +12753,10 @@
       <c r="B10" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="42" t="n">
+      <c r="C10" s="43" t="n">
         <v>191</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="43" t="s">
         <v>229</v>
       </c>
     </row>
@@ -12763,10 +12767,10 @@
       <c r="B11" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C11" s="42" t="n">
+      <c r="C11" s="43" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="43" t="s">
         <v>231</v>
       </c>
     </row>
@@ -12777,10 +12781,10 @@
       <c r="B12" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C12" s="42" t="n">
+      <c r="C12" s="43" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="43" t="s">
         <v>232</v>
       </c>
     </row>
@@ -12791,10 +12795,10 @@
       <c r="B13" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="42" t="n">
+      <c r="C13" s="43" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="44" t="s">
         <v>233</v>
       </c>
     </row>
@@ -12805,10 +12809,10 @@
       <c r="B14" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C14" s="42" t="n">
+      <c r="C14" s="43" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="43" t="s">
         <v>234</v>
       </c>
     </row>
@@ -12819,10 +12823,10 @@
       <c r="B15" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C15" s="42" t="n">
+      <c r="C15" s="43" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="44" t="s">
         <v>235</v>
       </c>
     </row>
@@ -12833,10 +12837,10 @@
       <c r="B16" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C16" s="42" t="n">
+      <c r="C16" s="43" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="44" t="s">
         <v>236</v>
       </c>
     </row>
@@ -12847,10 +12851,10 @@
       <c r="B17" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="42" t="n">
+      <c r="C17" s="43" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="44" t="s">
         <v>237</v>
       </c>
     </row>
@@ -12861,10 +12865,10 @@
       <c r="B18" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="C18" s="42" t="n">
+      <c r="C18" s="43" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="44" t="s">
         <v>238</v>
       </c>
     </row>
@@ -12875,10 +12879,10 @@
       <c r="B19" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C19" s="42" t="n">
+      <c r="C19" s="43" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="43" t="s">
         <v>240</v>
       </c>
     </row>
@@ -12889,10 +12893,10 @@
       <c r="B20" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C20" s="42" t="n">
+      <c r="C20" s="43" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="43" t="s">
         <v>241</v>
       </c>
     </row>
@@ -12903,10 +12907,10 @@
       <c r="B21" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C21" s="42" t="n">
+      <c r="C21" s="43" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="44" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12917,10 +12921,10 @@
       <c r="B22" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C22" s="42" t="n">
+      <c r="C22" s="43" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="43" t="s">
         <v>243</v>
       </c>
     </row>
@@ -12931,10 +12935,10 @@
       <c r="B23" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C23" s="42" t="n">
+      <c r="C23" s="43" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="44" t="s">
         <v>244</v>
       </c>
     </row>
@@ -12945,10 +12949,10 @@
       <c r="B24" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C24" s="42" t="n">
+      <c r="C24" s="43" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="44" t="s">
         <v>245</v>
       </c>
     </row>
@@ -12959,10 +12963,10 @@
       <c r="B25" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C25" s="42" t="n">
+      <c r="C25" s="43" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="44" t="s">
         <v>246</v>
       </c>
     </row>
@@ -12973,10 +12977,10 @@
       <c r="B26" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C26" s="42" t="n">
+      <c r="C26" s="43" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="44" t="s">
         <v>247</v>
       </c>
     </row>
@@ -12987,10 +12991,10 @@
       <c r="B27" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="42" t="n">
+      <c r="C27" s="43" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="43" t="s">
         <v>249</v>
       </c>
     </row>
@@ -13001,10 +13005,10 @@
       <c r="B28" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C28" s="42" t="n">
+      <c r="C28" s="43" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="43" t="s">
         <v>250</v>
       </c>
     </row>
@@ -13015,10 +13019,10 @@
       <c r="B29" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C29" s="42" t="n">
+      <c r="C29" s="43" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="45" t="s">
         <v>251</v>
       </c>
     </row>
@@ -13029,10 +13033,10 @@
       <c r="B30" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="42" t="n">
+      <c r="C30" s="43" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="43" t="s">
         <v>252</v>
       </c>
     </row>
@@ -13043,10 +13047,10 @@
       <c r="B31" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C31" s="42" t="n">
+      <c r="C31" s="43" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="44" t="s">
         <v>253</v>
       </c>
     </row>
@@ -13057,10 +13061,10 @@
       <c r="B32" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C32" s="42" t="n">
+      <c r="C32" s="43" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="44" t="s">
         <v>254</v>
       </c>
     </row>
@@ -13071,10 +13075,10 @@
       <c r="B33" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C33" s="42" t="n">
+      <c r="C33" s="43" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="44" t="s">
         <v>255</v>
       </c>
     </row>
@@ -13085,10 +13089,10 @@
       <c r="B34" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C34" s="42" t="n">
+      <c r="C34" s="43" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="44" t="s">
         <v>256</v>
       </c>
     </row>
@@ -13099,10 +13103,10 @@
       <c r="B35" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C35" s="42" t="n">
+      <c r="C35" s="43" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="42" t="n">
+      <c r="D35" s="43" t="n">
         <v>204</v>
       </c>
     </row>
@@ -13113,10 +13117,10 @@
       <c r="B36" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C36" s="42" t="n">
+      <c r="C36" s="43" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="42" t="n">
+      <c r="D36" s="43" t="n">
         <v>220</v>
       </c>
     </row>
@@ -13127,10 +13131,10 @@
       <c r="B37" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C37" s="42" t="n">
+      <c r="C37" s="43" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="43" t="n">
+      <c r="D37" s="44" t="n">
         <v>236</v>
       </c>
     </row>
@@ -13141,10 +13145,10 @@
       <c r="B38" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C38" s="42" t="n">
+      <c r="C38" s="43" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="42" t="n">
+      <c r="D38" s="43" t="n">
         <v>252</v>
       </c>
     </row>
@@ -13155,10 +13159,10 @@
       <c r="B39" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C39" s="42" t="n">
+      <c r="C39" s="43" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="43" t="n">
+      <c r="D39" s="44" t="n">
         <v>268</v>
       </c>
     </row>
@@ -13169,10 +13173,10 @@
       <c r="B40" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C40" s="42" t="n">
+      <c r="C40" s="43" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="43" t="n">
+      <c r="D40" s="44" t="n">
         <v>284</v>
       </c>
     </row>
@@ -13183,10 +13187,10 @@
       <c r="B41" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C41" s="42" t="n">
+      <c r="C41" s="43" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="43" t="n">
+      <c r="D41" s="44" t="n">
         <v>300</v>
       </c>
     </row>
@@ -13197,10 +13201,10 @@
       <c r="B42" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C42" s="42" t="n">
+      <c r="C42" s="43" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="43" t="n">
+      <c r="D42" s="44" t="n">
         <v>316</v>
       </c>
     </row>
@@ -13211,10 +13215,10 @@
       <c r="B43" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C43" s="42" t="n">
+      <c r="C43" s="43" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="42" t="n">
+      <c r="D43" s="43" t="n">
         <v>207</v>
       </c>
     </row>
@@ -13225,10 +13229,10 @@
       <c r="B44" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C44" s="42" t="n">
+      <c r="C44" s="43" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="42" t="n">
+      <c r="D44" s="43" t="n">
         <v>223</v>
       </c>
     </row>
@@ -13239,10 +13243,10 @@
       <c r="B45" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C45" s="42" t="n">
+      <c r="C45" s="43" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="43" t="n">
+      <c r="D45" s="44" t="n">
         <v>239</v>
       </c>
     </row>
@@ -13253,10 +13257,10 @@
       <c r="B46" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C46" s="42" t="n">
+      <c r="C46" s="43" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="42" t="n">
+      <c r="D46" s="43" t="n">
         <v>255</v>
       </c>
     </row>
@@ -13267,10 +13271,10 @@
       <c r="B47" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C47" s="42" t="n">
+      <c r="C47" s="43" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="43" t="n">
+      <c r="D47" s="44" t="n">
         <v>271</v>
       </c>
     </row>
@@ -13281,10 +13285,10 @@
       <c r="B48" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C48" s="42" t="n">
+      <c r="C48" s="43" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="43" t="n">
+      <c r="D48" s="44" t="n">
         <v>287</v>
       </c>
     </row>
@@ -13295,10 +13299,10 @@
       <c r="B49" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C49" s="42" t="n">
+      <c r="C49" s="43" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="43" t="n">
+      <c r="D49" s="44" t="n">
         <v>303</v>
       </c>
     </row>
@@ -13309,10 +13313,10 @@
       <c r="B50" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C50" s="42" t="n">
+      <c r="C50" s="43" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="43" t="n">
+      <c r="D50" s="44" t="n">
         <v>319</v>
       </c>
     </row>
@@ -14281,8 +14285,8 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:I10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14293,26 +14297,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>